<commit_message>
20230406 update : merge new model into old model.
</commit_message>
<xml_diff>
--- a/TestData/Book1.xlsx
+++ b/TestData/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\aspose\cells\cloud\src\testdata\Cells\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\test\data\asposecellscloudsdk\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAC6793-BD49-46ED-A252-75A83DDD28AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363DEB7A-E329-4687-BF50-318DFD33AB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,9 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet8" sheetId="9" r:id="rId7"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId8"/>
+    <sheet name="insert" sheetId="8" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet5!$B$3:$E$18</definedName>
@@ -38,6 +39,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -216,16 +218,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;¥&quot;* #,##0_ ;_ &quot;¥&quot;* \-#,##0_ ;_ &quot;¥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ &quot;¥&quot;* #,##0_ ;_ &quot;¥&quot;* \-#,##0_ ;_ &quot;¥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -239,7 +241,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -263,7 +265,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -295,37 +297,34 @@
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Comma" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Comma [0]" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Comma" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma [0]" xfId="5" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Currency" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Currency [0]" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Hyperlink" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Hyperlink" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Percent" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -410,7 +409,7 @@
               </a:solidFill>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -456,7 +455,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E9A9-49BF-9F9D-D855C1C2A88F}"/>
+              <c16:uniqueId val="{00000000-15C5-4825-96A1-5D2FC79E3257}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -497,7 +496,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E9A9-49BF-9F9D-D855C1C2A88F}"/>
+              <c16:uniqueId val="{00000001-15C5-4825-96A1-5D2FC79E3257}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -532,7 +531,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -577,12 +576,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-              <a:cs typeface="Calibri"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -676,7 +672,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-468D-470F-8F8A-009F6F20070C}"/>
+              <c16:uniqueId val="{00000000-CBA6-418D-A88C-293692B65FE7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -727,7 +723,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-468D-470F-8F8A-009F6F20070C}"/>
+              <c16:uniqueId val="{00000001-CBA6-418D-A88C-293692B65FE7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -741,12 +737,12 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:shape val="box"/>
-        <c:axId val="7764587"/>
-        <c:axId val="12186015"/>
+        <c:axId val="43572788"/>
+        <c:axId val="27656436"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="7764587"/>
+        <c:axId val="43572788"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -780,15 +776,12 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="Calibri"/>
-                <a:ea typeface="Calibri"/>
-                <a:cs typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12186015"/>
+        <c:crossAx val="27656436"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -796,7 +789,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="12186015"/>
+        <c:axId val="27656436"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -837,15 +830,12 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="Calibri"/>
-                <a:ea typeface="Calibri"/>
-                <a:cs typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7764587"/>
+        <c:crossAx val="43572788"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -882,7 +872,7 @@
               <a:cs typeface="Calibri"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -946,12 +936,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-              <a:cs typeface="Calibri"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1005,12 +992,9 @@
                         <a:lumOff val="25000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                    <a:ea typeface="Calibri"/>
-                    <a:cs typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="zh-CN"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -1115,7 +1099,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-DBFA-4A32-85D0-7EF9B0CF8DD1}"/>
+              <c16:uniqueId val="{00000000-081C-4415-9F2E-FE9C627FA749}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1166,11 +1150,11 @@
           </c:downBars>
         </c:upDownBars>
         <c:smooth val="0"/>
-        <c:axId val="63849291"/>
-        <c:axId val="56946769"/>
+        <c:axId val="56504966"/>
+        <c:axId val="41973208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63849291"/>
+        <c:axId val="56504966"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1204,15 +1188,12 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="Calibri"/>
-                <a:ea typeface="Calibri"/>
-                <a:cs typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56946769"/>
+        <c:crossAx val="41973208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1220,7 +1201,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56946769"/>
+        <c:axId val="41973208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1261,15 +1242,12 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="Calibri"/>
-                <a:ea typeface="Calibri"/>
-                <a:cs typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63849291"/>
+        <c:crossAx val="56504966"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1301,12 +1279,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="Calibri"/>
-                <a:ea typeface="Calibri"/>
-                <a:cs typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -1343,7 +1318,7 @@
               <a:cs typeface="Calibri"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1407,12 +1382,9 @@
                   <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-              <a:cs typeface="Calibri"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1469,7 +1441,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7957-443C-9D6D-A17F22CCF47D}"/>
+              <c16:uniqueId val="{00000000-D387-439A-8027-BD7B9BD07FA4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1520,7 +1492,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7957-443C-9D6D-A17F22CCF47D}"/>
+              <c16:uniqueId val="{00000001-D387-439A-8027-BD7B9BD07FA4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1571,7 +1543,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-7957-443C-9D6D-A17F22CCF47D}"/>
+              <c16:uniqueId val="{00000002-D387-439A-8027-BD7B9BD07FA4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1622,7 +1594,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-7957-443C-9D6D-A17F22CCF47D}"/>
+              <c16:uniqueId val="{00000003-D387-439A-8027-BD7B9BD07FA4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1635,11 +1607,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="23605975"/>
-        <c:axId val="34701889"/>
+        <c:axId val="9987539"/>
+        <c:axId val="59577537"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="23605975"/>
+        <c:axId val="9987539"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1673,15 +1645,12 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="Calibri"/>
-                <a:ea typeface="Calibri"/>
-                <a:cs typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34701889"/>
+        <c:crossAx val="59577537"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1689,7 +1658,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="34701889"/>
+        <c:axId val="59577537"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1730,15 +1699,12 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="Calibri"/>
-                <a:ea typeface="Calibri"/>
-                <a:cs typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23605975"/>
+        <c:crossAx val="9987539"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1775,7 +1741,7 @@
               <a:cs typeface="Calibri"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1850,7 +1816,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-368B-4702-9BDD-CA011A2E02A3}"/>
+              <c16:uniqueId val="{00000000-B875-4667-B1F2-1D275C079F40}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1878,7 +1844,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-368B-4702-9BDD-CA011A2E02A3}"/>
+              <c16:uniqueId val="{00000001-B875-4667-B1F2-1D275C079F40}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1892,11 +1858,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="4937521"/>
-        <c:axId val="25309069"/>
+        <c:axId val="3492865"/>
+        <c:axId val="50904140"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="4937521"/>
+        <c:axId val="3492865"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1909,7 +1875,7 @@
         <c:spPr>
           <a:ln w="9525" cap="flat" cmpd="sng"/>
         </c:spPr>
-        <c:crossAx val="25309069"/>
+        <c:crossAx val="50904140"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1917,7 +1883,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="25309069"/>
+        <c:axId val="50904140"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1931,7 +1897,7 @@
         <c:spPr>
           <a:ln w="9525" cap="flat" cmpd="sng"/>
         </c:spPr>
-        <c:crossAx val="4937521"/>
+        <c:crossAx val="3492865"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5156,8 +5122,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="2374498" y="60888"/>
-          <a:ext cx="917091" cy="797869"/>
+          <a:off x="2004230" y="67577"/>
+          <a:ext cx="1015751" cy="883704"/>
         </a:xfrm>
         <a:prstGeom prst="hexagon">
           <a:avLst>
@@ -5201,12 +5167,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="57150" tIns="57150" rIns="57150" bIns="57150" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="60960" tIns="60960" rIns="60960" bIns="60960" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="666750">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="711200">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5218,12 +5184,12 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1500" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="1600" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-5400000">
-        <a:off x="2558444" y="144190"/>
-        <a:ext cx="549199" cy="631265"/>
+        <a:off x="2207964" y="159842"/>
+        <a:ext cx="608282" cy="699175"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{B930369B-D2A0-4F63-9F48-D9B1B51F9A4E}">
@@ -5233,8 +5199,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3256190" y="184695"/>
-          <a:ext cx="1023473" cy="550254"/>
+          <a:off x="2980774" y="204704"/>
+          <a:ext cx="1133579" cy="609451"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5258,12 +5224,12 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="95250" tIns="95250" rIns="95250" bIns="95250" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="106680" tIns="106680" rIns="106680" bIns="106680" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="1111250">
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="1244600">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5275,12 +5241,12 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="en-US" sz="2500" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="2800" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3256190" y="184695"/>
-        <a:ext cx="1023473" cy="550254"/>
+        <a:off x="2980774" y="204704"/>
+        <a:ext cx="1133579" cy="609451"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{53337A83-2C88-47CB-8EA7-8DEB9E392E35}">
@@ -5290,8 +5256,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="1512799" y="60888"/>
-          <a:ext cx="917091" cy="797869"/>
+          <a:off x="1049829" y="67577"/>
+          <a:ext cx="1015751" cy="883704"/>
         </a:xfrm>
         <a:prstGeom prst="hexagon">
           <a:avLst>
@@ -5356,8 +5322,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-5400000">
-        <a:off x="1696745" y="144190"/>
-        <a:ext cx="549199" cy="631265"/>
+        <a:off x="1253563" y="159842"/>
+        <a:ext cx="608282" cy="699175"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{647BCE6B-49D9-4061-808E-497371A775C8}">
@@ -5367,8 +5333,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="1941998" y="839315"/>
-          <a:ext cx="917091" cy="797869"/>
+          <a:off x="1525201" y="929747"/>
+          <a:ext cx="1015751" cy="883704"/>
         </a:xfrm>
         <a:prstGeom prst="hexagon">
           <a:avLst>
@@ -5412,12 +5378,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="57150" tIns="57150" rIns="57150" bIns="57150" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="60960" tIns="60960" rIns="60960" bIns="60960" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="666750">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="711200">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5429,12 +5395,12 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1500" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="1600" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-5400000">
-        <a:off x="2125944" y="922617"/>
-        <a:ext cx="549199" cy="631265"/>
+        <a:off x="1728935" y="1022012"/>
+        <a:ext cx="608282" cy="699175"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{E69DED3E-1798-498A-B9A6-EC95C7494A6D}">
@@ -5444,8 +5410,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="978135" y="963122"/>
-          <a:ext cx="990458" cy="550254"/>
+          <a:off x="457646" y="1066874"/>
+          <a:ext cx="1097012" cy="609451"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5469,12 +5435,12 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="95250" tIns="95250" rIns="95250" bIns="95250" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="106680" tIns="106680" rIns="106680" bIns="106680" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="r" defTabSz="1111250">
+          <a:pPr marL="0" lvl="0" indent="0" algn="r" defTabSz="1244600">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5486,12 +5452,12 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="en-US" sz="2500" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="2800" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="978135" y="963122"/>
-        <a:ext cx="990458" cy="550254"/>
+        <a:off x="457646" y="1066874"/>
+        <a:ext cx="1097012" cy="609451"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{8FC7D08A-84F9-4114-9F68-EAA65B3092AA}">
@@ -5501,8 +5467,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="2803697" y="839315"/>
-          <a:ext cx="917091" cy="797869"/>
+          <a:off x="2479602" y="929747"/>
+          <a:ext cx="1015751" cy="883704"/>
         </a:xfrm>
         <a:prstGeom prst="hexagon">
           <a:avLst>
@@ -5567,8 +5533,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-5400000">
-        <a:off x="2987643" y="922617"/>
-        <a:ext cx="549199" cy="631265"/>
+        <a:off x="2683336" y="1022012"/>
+        <a:ext cx="608282" cy="699175"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{B7F626B2-5CA0-4456-B060-5D90A1C6F809}">
@@ -5578,8 +5544,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="2374498" y="1617742"/>
-          <a:ext cx="917091" cy="797869"/>
+          <a:off x="2004230" y="1791918"/>
+          <a:ext cx="1015751" cy="883704"/>
         </a:xfrm>
         <a:prstGeom prst="hexagon">
           <a:avLst>
@@ -5623,12 +5589,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="57150" tIns="57150" rIns="57150" bIns="57150" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="60960" tIns="60960" rIns="60960" bIns="60960" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="666750">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="711200">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5640,12 +5606,12 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1500" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="1600" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-5400000">
-        <a:off x="2558444" y="1701044"/>
-        <a:ext cx="549199" cy="631265"/>
+        <a:off x="2207964" y="1884183"/>
+        <a:ext cx="608282" cy="699175"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{F941179A-7E65-4142-A4DE-C77422569540}">
@@ -5655,8 +5621,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3256190" y="1741549"/>
-          <a:ext cx="1023473" cy="550254"/>
+          <a:off x="2980774" y="1929044"/>
+          <a:ext cx="1133579" cy="609451"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5680,12 +5646,12 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="95250" tIns="95250" rIns="95250" bIns="95250" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="106680" tIns="106680" rIns="106680" bIns="106680" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="1111250">
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="1244600">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5697,12 +5663,12 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="en-US" sz="2500" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="2800" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3256190" y="1741549"/>
-        <a:ext cx="1023473" cy="550254"/>
+        <a:off x="2980774" y="1929044"/>
+        <a:ext cx="1133579" cy="609451"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{E548E58E-B118-4D34-9B17-B7C7F1C4A379}">
@@ -5712,8 +5678,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="1512799" y="1617742"/>
-          <a:ext cx="917091" cy="797869"/>
+          <a:off x="1049829" y="1791918"/>
+          <a:ext cx="1015751" cy="883704"/>
         </a:xfrm>
         <a:prstGeom prst="hexagon">
           <a:avLst>
@@ -5778,8 +5744,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-5400000">
-        <a:off x="1696745" y="1701044"/>
-        <a:ext cx="549199" cy="631265"/>
+        <a:off x="1253563" y="1884183"/>
+        <a:ext cx="608282" cy="699175"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -5801,8 +5767,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="0" y="327810"/>
-          <a:ext cx="5257800" cy="453600"/>
+          <a:off x="0" y="359999"/>
+          <a:ext cx="4572000" cy="504000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5849,8 +5815,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="262890" y="62130"/>
-          <a:ext cx="3680460" cy="531360"/>
+          <a:off x="228600" y="64799"/>
+          <a:ext cx="3200400" cy="590400"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -5891,12 +5857,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="139113" tIns="0" rIns="139113" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="120968" tIns="0" rIns="120968" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="800100">
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5908,12 +5874,12 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1800" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="2000" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="288829" y="88069"/>
-        <a:ext cx="3628582" cy="479482"/>
+        <a:off x="257421" y="93620"/>
+        <a:ext cx="3142758" cy="532758"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{9A40B308-CE02-4B71-BA70-C0D200CBD383}">
@@ -5923,8 +5889,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="0" y="1144290"/>
-          <a:ext cx="5257800" cy="453600"/>
+          <a:off x="0" y="1267200"/>
+          <a:ext cx="4572000" cy="504000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5971,8 +5937,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="262890" y="878610"/>
-          <a:ext cx="3680460" cy="531360"/>
+          <a:off x="228600" y="972000"/>
+          <a:ext cx="3200400" cy="590400"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -6013,12 +5979,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="139113" tIns="0" rIns="139113" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="120968" tIns="0" rIns="120968" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="800100">
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6030,12 +5996,12 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1800" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="2000" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="288829" y="904549"/>
-        <a:ext cx="3628582" cy="479482"/>
+        <a:off x="257421" y="1000821"/>
+        <a:ext cx="3142758" cy="532758"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{BE4CD07D-369F-49DD-8139-FD09651870C8}">
@@ -6045,8 +6011,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="0" y="1960770"/>
-          <a:ext cx="5257800" cy="453600"/>
+          <a:off x="0" y="2174400"/>
+          <a:ext cx="4572000" cy="504000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6093,8 +6059,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="262890" y="1695090"/>
-          <a:ext cx="3680460" cy="531360"/>
+          <a:off x="228600" y="1879200"/>
+          <a:ext cx="3200400" cy="590400"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -6135,12 +6101,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="139113" tIns="0" rIns="139113" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="120968" tIns="0" rIns="120968" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="800100">
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6152,12 +6118,12 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1800" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="2000" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="288829" y="1721029"/>
-        <a:ext cx="3628582" cy="479482"/>
+        <a:off x="257421" y="1908021"/>
+        <a:ext cx="3142758" cy="532758"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -11359,23 +11325,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C9FAE5B-687B-188C-0EA2-F6CADF7C07A8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{941E4FC8-CC1D-4230-B574-74FEBC8A88D2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11397,8 +11363,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="685800" y="342900"/>
-          <a:ext cx="3552825" cy="1733550"/>
+          <a:off x="409575" y="514350"/>
+          <a:ext cx="3171825" cy="1924050"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11764,11 +11730,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="2:20">
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
     </row>
     <row r="3" spans="2:20">
       <c r="B3">
@@ -11798,8 +11764,8 @@
       </c>
     </row>
     <row r="7" spans="2:20">
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
     </row>
     <row r="11" spans="2:20">
       <c r="D11">
@@ -11807,62 +11773,62 @@
       </c>
     </row>
     <row r="13" spans="2:20">
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
     </row>
     <row r="14" spans="2:20">
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
     </row>
     <row r="15" spans="2:20">
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
     </row>
     <row r="16" spans="2:20">
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
     </row>
     <row r="17" spans="18:20">
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
     </row>
     <row r="18" spans="18:20">
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
     </row>
     <row r="19" spans="18:20">
-      <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
-      <c r="T19" s="8"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
     </row>
     <row r="35" spans="5:5">
-      <c r="E35" s="1" t="s">
+      <c r="E35" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="5:5">
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="5:5">
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="38" spans="5:5">
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="39" spans="5:5">
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -11891,7 +11857,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30:G34 I34:J35 M35 L35:L36 L38 J41 F41">
-    <cfRule type="dataBar" priority="7">
+    <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11972,44 +11938,44 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="7" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:8">
-      <c r="C5" s="3"/>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
     </row>
-    <row r="8" spans="2:8" ht="14.25">
+    <row r="8" spans="2:8">
       <c r="G8" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:8">
       <c r="F10" s="4">
         <f ca="1">NOW()</f>
-        <v>44706.569663657407</v>
+        <v>44939.719515277779</v>
       </c>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
     </row>
     <row r="14" spans="2:8">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -12028,7 +11994,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="15" spans="5:6">
       <c r="E15" t="s">
@@ -12100,7 +12066,7 @@
   <sheetViews>
     <sheetView topLeftCell="B43" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="7" spans="3:4">
       <c r="C7" t="s">
@@ -12158,9 +12124,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5">
@@ -12413,7 +12379,7 @@
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScale="50" zoomScaleNormal="50" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="3" spans="19:29"/>
     <row r="13" spans="19:29">
@@ -12550,15 +12516,28 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C802F16A-C50B-482A-860E-AEA43686CD41}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="C3:P23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="9" width="10.875" customWidth="1"/>
-    <col min="13" max="16" width="10.875" customWidth="1"/>
+    <col min="3" max="9" width="10.85546875" customWidth="1"/>
+    <col min="13" max="16" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:16">
@@ -12652,10 +12631,10 @@
       <c r="I6">
         <v>3</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="M6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="N6" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O6" t="s">
@@ -12687,8 +12666,8 @@
       <c r="I7">
         <v>4</v>
       </c>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
     </row>
     <row r="8" spans="3:16">
       <c r="C8">
@@ -12712,8 +12691,8 @@
       <c r="I8">
         <v>5</v>
       </c>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
     </row>
     <row r="9" spans="3:16">
       <c r="C9">
@@ -12737,8 +12716,8 @@
       <c r="I9">
         <v>6</v>
       </c>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
     </row>
     <row r="10" spans="3:16">
       <c r="C10">
@@ -12762,8 +12741,8 @@
       <c r="I10">
         <v>7</v>
       </c>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
     </row>
     <row r="11" spans="3:16">
       <c r="C11">
@@ -13076,18 +13055,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{829CF65E-34BA-43EF-84E2-8CC1ACB62A83}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>